<commit_message>
Enhanced batch list page with filters and batch ID column
- Added Batch ID column for easy student import identification
- Fixed all filter functionality (Course, Status, Branch filters)
- Improved timing display with proper formatting
- Fixed 'Clear All Filters' function and button functionality
- Enhanced CSS styling for batch ID badges and timing display
- Added debugging functions for troubleshooting
- Resolved DataTables column indexing issues after adding Batch ID
- Improved filter logic to handle HTML content properly
</commit_message>
<xml_diff>
--- a/Course_Master___12_Programs.xlsx
+++ b/Course_Master___12_Programs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/78d7c3c817fab242/Documents/01 GLOBAL IT/LMS/Course Brochers/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\globalitwebapp2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FED721EC-8E85-46AB-A594-8A67A1DE1A22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CE4D67E-832B-4289-8002-32714745FA71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Course_Master___12_Programs" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="146">
   <si>
     <t>course_name</t>
   </si>
@@ -777,11 +777,23 @@
 AI Coaching for Speech Practice
 Final Leadership Speech &amp; Portfolio</t>
   </si>
+  <si>
+    <t>Canva for Beginners</t>
+  </si>
+  <si>
+    <t>CANFOR</t>
+  </si>
+  <si>
+    <t>Graphic Design</t>
+  </si>
+  <si>
+    <t>1 Month</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1601,11 +1613,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Z14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" topLeftCell="C10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="X14" sqref="X14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2658,6 +2670,65 @@
         <v>40</v>
       </c>
     </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>142</v>
+      </c>
+      <c r="B14" t="s">
+        <v>143</v>
+      </c>
+      <c r="C14" t="s">
+        <v>144</v>
+      </c>
+      <c r="D14" t="s">
+        <v>145</v>
+      </c>
+      <c r="E14">
+        <v>26</v>
+      </c>
+      <c r="F14">
+        <v>30</v>
+      </c>
+      <c r="G14">
+        <v>6500</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>5</v>
+      </c>
+      <c r="R14">
+        <v>16</v>
+      </c>
+      <c r="S14" t="s">
+        <v>35</v>
+      </c>
+      <c r="T14" t="s">
+        <v>36</v>
+      </c>
+      <c r="U14" t="s">
+        <v>117</v>
+      </c>
+      <c r="V14" t="s">
+        <v>38</v>
+      </c>
+      <c r="W14" t="s">
+        <v>35</v>
+      </c>
+      <c r="X14" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y14">
+        <v>13</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>